<commit_message>
added way to get prediction for new cases from github
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding_new.xlsx
+++ b/lsh_data_processing/lsh_coding_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Signy/Projects/covid/BCS1/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6126895-D020-314D-B110-7621F4027F91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BCA75F-D0DF-0B4D-8ED4-7D57C48D02E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23880" windowHeight="17540" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="346">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -1071,6 +1071,9 @@
   </si>
   <si>
     <t>Félagsráðgjöf</t>
+  </si>
+  <si>
+    <t>Kl-1h GD Kleppi</t>
   </si>
 </sst>
 </file>
@@ -6448,10 +6451,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8857,6 +8860,23 @@
         <v>10</v>
       </c>
       <c r="E141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="B142" t="s">
+        <v>31</v>
+      </c>
+      <c r="C142" t="s">
+        <v>35</v>
+      </c>
+      <c r="D142" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding option to hide IC
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding_new.xlsx
+++ b/lsh_data_processing/lsh_coding_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Signy/Projects/covid/BCS1/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5791226E-1AE9-4245-953C-C34722937EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2596635A-E905-D949-9657-FC5CC9AB00C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23880" windowHeight="17540" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="351">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -1083,6 +1083,12 @@
   </si>
   <si>
     <t>Öldrunarlækningadeild B (Lk-K2)</t>
+  </si>
+  <si>
+    <t>Hb-10E GD Kviðarhols- og brjóstaskurðlækninga, deildarlæknar</t>
+  </si>
+  <si>
+    <t>Hb-23E DD Barna BH</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1219,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1226,7 +1232,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6463,8 +6468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8942,10 +8947,38 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="7"/>
+      <c r="A146" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B146" t="s">
+        <v>31</v>
+      </c>
+      <c r="C146" t="s">
+        <v>35</v>
+      </c>
+      <c r="D146" t="s">
+        <v>10</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="8"/>
+      <c r="A147" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B147" t="s">
+        <v>141</v>
+      </c>
+      <c r="C147" t="s">
+        <v>35</v>
+      </c>
+      <c r="D147" t="s">
+        <v>10</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
manually select hospital prob
</commit_message>
<xml_diff>
--- a/lsh_data_processing/lsh_coding_new.xlsx
+++ b/lsh_data_processing/lsh_coding_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Signy/Projects/covid/BCS/lsh_data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A371F458-FA84-3247-936C-7E00D41F386C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE078331-05F8-9F49-A4C7-7351B7138271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23880" windowHeight="17540" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23880" windowHeight="17500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lsh_covid_groups" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="386">
   <si>
     <t>text_out_category_raw</t>
   </si>
@@ -1092,6 +1092,108 @@
   </si>
   <si>
     <t>COVID-19 einangrun aflétt</t>
+  </si>
+  <si>
+    <t>Hb-11F GD Sálfræðiþjónusta</t>
+  </si>
+  <si>
+    <t>Kv-H8 GD Líknardeildar</t>
+  </si>
+  <si>
+    <t>Hb-14D GD Sjúkraþjálfun H</t>
+  </si>
+  <si>
+    <t>La71 GD Laugarásinn meðferðargeðdeild</t>
+  </si>
+  <si>
+    <t>Fv-B1 GD Iðjuþjálfun F</t>
+  </si>
+  <si>
+    <t>Gr-R3 DD Endurhæfingar</t>
+  </si>
+  <si>
+    <t>Gr-R3 GD Læknar endurhæfingar</t>
+  </si>
+  <si>
+    <t>Ei5 GD Augnlækninga</t>
+  </si>
+  <si>
+    <t>Ei5 GD Innkirtla- og efnaskipta</t>
+  </si>
+  <si>
+    <t>Sjúkrahótel Landspítala (Hb-4)</t>
+  </si>
+  <si>
+    <t>Ei5 GD Gigtarlækninga</t>
+  </si>
+  <si>
+    <t>Gr-R1 GD Sjúkraþjálfun G</t>
+  </si>
+  <si>
+    <t>Fv-B7 DD Alm.lyflækninga</t>
+  </si>
+  <si>
+    <t>Öldrunarlækningadeild (Lk-L5)</t>
+  </si>
+  <si>
+    <t>Ei5 GD Erfða- og sameindalæknisfræðideild</t>
+  </si>
+  <si>
+    <t>Ei5 DD Gigtarlækningar</t>
+  </si>
+  <si>
+    <t>Ei5 GD Sálfræðiþjónusta</t>
+  </si>
+  <si>
+    <t>Fv-E4 Æðaþræðing-inngripsröntgen</t>
+  </si>
+  <si>
+    <t>Ei5 GD Brjóstamóttaka</t>
+  </si>
+  <si>
+    <t>Ei5 GD Lýtalækninga</t>
+  </si>
+  <si>
+    <t>Næringarstofa</t>
+  </si>
+  <si>
+    <t>Hs-7h GD Verkjamiðstöð</t>
+  </si>
+  <si>
+    <t>Hb-20E Næringarstofa BH</t>
+  </si>
+  <si>
+    <t>Ei5 GD Krabbameins</t>
+  </si>
+  <si>
+    <t>Ei5 GD Kviðarhols- og brjóstaskurðlækninga</t>
+  </si>
+  <si>
+    <t>Fv-Bb DD Lyflækningaþjónusta</t>
+  </si>
+  <si>
+    <t>Kl-Sk SV Samfélagsgeðteymi</t>
+  </si>
+  <si>
+    <t>Fv-B3 GD Talmeinaþjónusta</t>
+  </si>
+  <si>
+    <t>Hb-10D GD Hjartavísindarannsóknir</t>
+  </si>
+  <si>
+    <t>Db12-0h Iðjuþjálfun geðendurhæfing</t>
+  </si>
+  <si>
+    <t>Kl-H10 DD Iðjuþjálfunar Kleppi</t>
+  </si>
+  <si>
+    <t>Fv-G3 GD SBS - inniliggjandi</t>
+  </si>
+  <si>
+    <t>Hb-20E GD Talmeinaþjónusta BH</t>
+  </si>
+  <si>
+    <t>Hb-21A GD Innskriftir kvenna</t>
   </si>
 </sst>
 </file>
@@ -6397,8 +6499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F531C9-8D09-6E45-B72D-D7F85CF9D0F7}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6480,10 +6582,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8991,6 +9093,584 @@
         <v>10</v>
       </c>
       <c r="E147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B148" t="s">
+        <v>141</v>
+      </c>
+      <c r="C148" t="s">
+        <v>35</v>
+      </c>
+      <c r="D148" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B149" t="s">
+        <v>141</v>
+      </c>
+      <c r="C149" t="s">
+        <v>35</v>
+      </c>
+      <c r="D149" t="s">
+        <v>10</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>354</v>
+      </c>
+      <c r="B150" t="s">
+        <v>31</v>
+      </c>
+      <c r="C150" t="s">
+        <v>35</v>
+      </c>
+      <c r="D150" t="s">
+        <v>10</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>355</v>
+      </c>
+      <c r="B151" t="s">
+        <v>31</v>
+      </c>
+      <c r="C151" t="s">
+        <v>35</v>
+      </c>
+      <c r="D151" t="s">
+        <v>10</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B152" t="s">
+        <v>31</v>
+      </c>
+      <c r="C152" t="s">
+        <v>35</v>
+      </c>
+      <c r="D152" t="s">
+        <v>10</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B153" t="s">
+        <v>141</v>
+      </c>
+      <c r="C153" t="s">
+        <v>35</v>
+      </c>
+      <c r="D153" t="s">
+        <v>10</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B154" t="s">
+        <v>31</v>
+      </c>
+      <c r="C154" t="s">
+        <v>35</v>
+      </c>
+      <c r="D154" t="s">
+        <v>10</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>359</v>
+      </c>
+      <c r="B155" t="s">
+        <v>31</v>
+      </c>
+      <c r="C155" t="s">
+        <v>35</v>
+      </c>
+      <c r="D155" t="s">
+        <v>10</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>360</v>
+      </c>
+      <c r="B156" t="s">
+        <v>31</v>
+      </c>
+      <c r="C156" t="s">
+        <v>35</v>
+      </c>
+      <c r="D156" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>361</v>
+      </c>
+      <c r="B157" t="s">
+        <v>30</v>
+      </c>
+      <c r="C157" t="s">
+        <v>34</v>
+      </c>
+      <c r="D157" t="s">
+        <v>34</v>
+      </c>
+      <c r="E157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>362</v>
+      </c>
+      <c r="B158" t="s">
+        <v>31</v>
+      </c>
+      <c r="C158" t="s">
+        <v>35</v>
+      </c>
+      <c r="D158" t="s">
+        <v>10</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>363</v>
+      </c>
+      <c r="B159" t="s">
+        <v>31</v>
+      </c>
+      <c r="C159" t="s">
+        <v>35</v>
+      </c>
+      <c r="D159" t="s">
+        <v>10</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>364</v>
+      </c>
+      <c r="B160" t="s">
+        <v>141</v>
+      </c>
+      <c r="C160" t="s">
+        <v>35</v>
+      </c>
+      <c r="D160" t="s">
+        <v>10</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>365</v>
+      </c>
+      <c r="B161" t="s">
+        <v>30</v>
+      </c>
+      <c r="C161" t="s">
+        <v>61</v>
+      </c>
+      <c r="D161" t="s">
+        <v>34</v>
+      </c>
+      <c r="E161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>366</v>
+      </c>
+      <c r="B162" t="s">
+        <v>31</v>
+      </c>
+      <c r="C162" t="s">
+        <v>35</v>
+      </c>
+      <c r="D162" t="s">
+        <v>10</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>367</v>
+      </c>
+      <c r="B163" t="s">
+        <v>141</v>
+      </c>
+      <c r="C163" t="s">
+        <v>35</v>
+      </c>
+      <c r="D163" t="s">
+        <v>10</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>368</v>
+      </c>
+      <c r="B164" t="s">
+        <v>31</v>
+      </c>
+      <c r="C164" t="s">
+        <v>35</v>
+      </c>
+      <c r="D164" t="s">
+        <v>10</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>369</v>
+      </c>
+      <c r="B165" t="s">
+        <v>31</v>
+      </c>
+      <c r="C165" t="s">
+        <v>35</v>
+      </c>
+      <c r="D165" t="s">
+        <v>10</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>370</v>
+      </c>
+      <c r="B166" t="s">
+        <v>31</v>
+      </c>
+      <c r="C166" t="s">
+        <v>35</v>
+      </c>
+      <c r="D166" t="s">
+        <v>10</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>371</v>
+      </c>
+      <c r="B167" t="s">
+        <v>31</v>
+      </c>
+      <c r="C167" t="s">
+        <v>35</v>
+      </c>
+      <c r="D167" t="s">
+        <v>10</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>372</v>
+      </c>
+      <c r="B168" t="s">
+        <v>31</v>
+      </c>
+      <c r="C168" t="s">
+        <v>35</v>
+      </c>
+      <c r="D168" t="s">
+        <v>10</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>373</v>
+      </c>
+      <c r="B169" t="s">
+        <v>31</v>
+      </c>
+      <c r="C169" t="s">
+        <v>35</v>
+      </c>
+      <c r="D169" t="s">
+        <v>10</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>374</v>
+      </c>
+      <c r="B170" t="s">
+        <v>31</v>
+      </c>
+      <c r="C170" t="s">
+        <v>35</v>
+      </c>
+      <c r="D170" t="s">
+        <v>10</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>375</v>
+      </c>
+      <c r="B171" t="s">
+        <v>31</v>
+      </c>
+      <c r="C171" t="s">
+        <v>35</v>
+      </c>
+      <c r="D171" t="s">
+        <v>10</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>376</v>
+      </c>
+      <c r="B172" t="s">
+        <v>31</v>
+      </c>
+      <c r="C172" t="s">
+        <v>35</v>
+      </c>
+      <c r="D172" t="s">
+        <v>10</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>377</v>
+      </c>
+      <c r="B173" t="s">
+        <v>141</v>
+      </c>
+      <c r="C173" t="s">
+        <v>35</v>
+      </c>
+      <c r="D173" t="s">
+        <v>10</v>
+      </c>
+      <c r="E173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>378</v>
+      </c>
+      <c r="B174" t="s">
+        <v>31</v>
+      </c>
+      <c r="C174" t="s">
+        <v>35</v>
+      </c>
+      <c r="D174" t="s">
+        <v>10</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>379</v>
+      </c>
+      <c r="B175" t="s">
+        <v>31</v>
+      </c>
+      <c r="C175" t="s">
+        <v>35</v>
+      </c>
+      <c r="D175" t="s">
+        <v>10</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>380</v>
+      </c>
+      <c r="B176" t="s">
+        <v>31</v>
+      </c>
+      <c r="C176" t="s">
+        <v>35</v>
+      </c>
+      <c r="D176" t="s">
+        <v>10</v>
+      </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>381</v>
+      </c>
+      <c r="B177" t="s">
+        <v>31</v>
+      </c>
+      <c r="C177" t="s">
+        <v>35</v>
+      </c>
+      <c r="D177" t="s">
+        <v>10</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>382</v>
+      </c>
+      <c r="B178" t="s">
+        <v>141</v>
+      </c>
+      <c r="C178" t="s">
+        <v>35</v>
+      </c>
+      <c r="D178" t="s">
+        <v>10</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>383</v>
+      </c>
+      <c r="B179" t="s">
+        <v>31</v>
+      </c>
+      <c r="C179" t="s">
+        <v>35</v>
+      </c>
+      <c r="D179" t="s">
+        <v>10</v>
+      </c>
+      <c r="E179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>384</v>
+      </c>
+      <c r="B180" t="s">
+        <v>31</v>
+      </c>
+      <c r="C180" t="s">
+        <v>35</v>
+      </c>
+      <c r="D180" t="s">
+        <v>10</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>385</v>
+      </c>
+      <c r="B181" t="s">
+        <v>31</v>
+      </c>
+      <c r="C181" t="s">
+        <v>35</v>
+      </c>
+      <c r="D181" t="s">
+        <v>10</v>
+      </c>
+      <c r="E181">
         <v>1</v>
       </c>
     </row>

</xml_diff>